<commit_message>
Updating for adjusted HW design.
</commit_message>
<xml_diff>
--- a/Firmware/Resources/CanBusSpeed.xlsx
+++ b/Firmware/Resources/CanBusSpeed.xlsx
@@ -506,6 +506,9 @@
     <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -517,13 +520,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -923,11 +923,11 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="23">
         <f>E8</f>
         <v>4.8543689320388345E-3</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="23"/>
       <c r="E8" s="10">
         <f>MIN(F8,G8)</f>
         <v>4.8543689320388345E-3</v>
@@ -1198,12 +1198,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="19">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="10">
         <f>B1*1000000</f>
-        <v>8000000</v>
+        <v>48000000</v>
       </c>
       <c r="F1" s="10"/>
     </row>
@@ -1211,10 +1211,10 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="26">
         <v>125</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="E2" s="10">
         <f>B2*1000</f>
         <v>125000</v>
@@ -1240,10 +1240,10 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="25">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="25"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="2"/>
@@ -1286,11 +1286,11 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="23">
         <f>E8</f>
         <v>4.8543689320388345E-3</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="23"/>
       <c r="E8" s="10">
         <f>MIN(F8,G8)</f>
         <v>4.8543689320388345E-3</v>
@@ -1312,14 +1312,14 @@
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="24">
         <f>CEILING(E10,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C10" s="23"/>
+        <v>11</v>
+      </c>
+      <c r="C10" s="24"/>
       <c r="E10" s="10">
         <f>FREQUENCY/(2*TQ*BITRATE_DESIRED)-1</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -1537,7 +1537,10 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -1547,8 +1550,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
@@ -1622,7 +1623,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="13">
         <v>5000</v>
       </c>
@@ -1656,22 +1657,22 @@
       <c r="C3" s="9">
         <v>20</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="9">
         <v>16</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
         <v>16</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="9">
         <v>16</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="9">
         <v>16</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="9">
         <v>10</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="9">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed CAN bus timings.
</commit_message>
<xml_diff>
--- a/Firmware/Resources/CanBusSpeed.xlsx
+++ b/Firmware/Resources/CanBusSpeed.xlsx
@@ -14,32 +14,32 @@
   <definedNames>
     <definedName name="BITRATE">BRP!$E$6</definedName>
     <definedName name="BITRATE_DESIRED">BRP!$E$2</definedName>
-    <definedName name="BRP">BRP!$B$11</definedName>
-    <definedName name="BUS_PROPAGATION_DELAY">BRP!$E$23</definedName>
+    <definedName name="BRP">BRP!$B$12</definedName>
+    <definedName name="BUS_PROPAGATION_DELAY">BRP!$E$24</definedName>
     <definedName name="FREQUENCY">BRP!$E$1</definedName>
     <definedName name="LENGTH">BRP!$B$3</definedName>
     <definedName name="OSC_TOLERANCE">BRP!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Bitrate!$A$1:$C$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">BRP!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">BRP!$A$1:$C$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'CiA DS-102'!$A$1:$I$8</definedName>
-    <definedName name="PROPAGATION_TIME">BRP!$E$19</definedName>
+    <definedName name="PROPAGATION_TIME">BRP!$E$20</definedName>
     <definedName name="PROPAGATION_TIME_DESIRED">BRP!$E$3</definedName>
-    <definedName name="PRSEG_TQ">BRP!$F$12</definedName>
-    <definedName name="SEG1PH_TQ">BRP!$E$13</definedName>
-    <definedName name="SEG2PH_TQ">BRP!$E$14</definedName>
-    <definedName name="SJW_TQ">BRP!$E$15</definedName>
-    <definedName name="TBIT_TIME">BRP!$E$18</definedName>
+    <definedName name="PRSEG_TQ">BRP!$E$13</definedName>
+    <definedName name="SEG1PH_TQ">BRP!$E$14</definedName>
+    <definedName name="SEG2PH_TQ">BRP!$E$15</definedName>
+    <definedName name="SJW_TQ">BRP!$E$16</definedName>
+    <definedName name="TBIT_TIME">BRP!$E$19</definedName>
     <definedName name="TQ">BRP!$B$4</definedName>
-    <definedName name="TQ_TIME">BRP!$E$17</definedName>
-    <definedName name="TRANSCEIVER_DELAY">BRP!$E$24</definedName>
-    <definedName name="VRP">BRP!$B$11</definedName>
+    <definedName name="TQ_TIME">BRP!$E$18</definedName>
+    <definedName name="TRANSCEIVER_DELAY">BRP!$E$25</definedName>
+    <definedName name="VRP">BRP!$B$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>BRP:</t>
   </si>
@@ -307,6 +307,58 @@
   </si>
   <si>
     <t>Bitrate error:</t>
+  </si>
+  <si>
+    <r>
+      <t>Real T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Desired T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -320,7 +372,7 @@
     <numFmt numFmtId="167" formatCode="0\ &quot;kbps&quot;"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;m&quot;"/>
     <numFmt numFmtId="169" formatCode="#,##0\ &quot;m&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.0000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -443,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -524,20 +576,161 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1186,7 +1379,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
@@ -1198,10 +1391,10 @@
     <col min="2" max="3" width="5.77734375" customWidth="1"/>
     <col min="5" max="6" width="10.77734375" style="11" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1215,7 +1408,7 @@
       </c>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1422,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1244,9 +1437,9 @@
       <c r="F3" s="10"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B4" s="26">
         <v>16</v>
@@ -1256,11 +1449,11 @@
       <c r="F4" s="10"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1275,207 +1468,218 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="27">
         <f>BITRATE/BITRATE_DESIRED-1</f>
         <v>0</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="27"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="22">
         <f>E8</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="C8" s="22"/>
       <c r="E8" s="10">
+        <f>ROUNDDOWN(F8,-(FLOOR(LOG10(F8),1)))</f>
+        <v>600</v>
+      </c>
+      <c r="F8" s="10">
         <f>ROUND((PROPAGATION_TIME-TRANSCEIVER_DELAY)/BUS_PROPAGATION_DELAY,0)</f>
         <v>650</v>
       </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="23">
         <f>E9</f>
-        <v>4.8543689320388345E-3</v>
+        <v>3.1250000000000002E-3</v>
       </c>
       <c r="C9" s="23"/>
       <c r="E9" s="10">
         <f>MIN(F9,G9)</f>
-        <v>4.8543689320388345E-3</v>
+        <v>3.1250000000000002E-3</v>
       </c>
       <c r="F9" s="10">
         <f>SJW_TQ/(20*TQ)</f>
-        <v>6.2500000000000003E-3</v>
+        <v>3.1250000000000002E-3</v>
       </c>
       <c r="G9" s="1">
         <f>MIN(SEG1PH_TQ, SEG2PH_TQ) / (2*(13*TQ-SEG2PH_TQ))</f>
         <v>4.8543689320388345E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="31">
+        <f>PRSEG_TQ+SEG1PH_TQ+SEG2PH_TQ+SJW_TQ</f>
+        <v>16</v>
+      </c>
+      <c r="C10" s="31"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="25">
-        <f>CEILING(E11,1)</f>
+      <c r="B12" s="25">
+        <f>CEILING(E12,1)</f>
         <v>11</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="E11" s="10">
+      <c r="C12" s="25"/>
+      <c r="E12" s="10">
         <f>FREQUENCY/(2*TQ*BITRATE_DESIRED)-1</f>
         <v>11</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4">
-        <f>E12-1</f>
-        <v>5</v>
-      </c>
-      <c r="C12" s="8" t="str">
-        <f>VLOOKUP(B12,E26:F33,2)</f>
-        <v>6 TQ</v>
-      </c>
-      <c r="E12" s="1">
-        <f>TQ-SEG1PH_TQ-SEG2PH_TQ-SJW_TQ</f>
+      <c r="B13" s="4">
+        <f>PRSEG_TQ-1</f>
         <v>6</v>
       </c>
-      <c r="F12" s="1">
-        <f>MAX(G12,H12)</f>
+      <c r="C13" s="8" t="str">
+        <f>VLOOKUP(B13,E27:F34,2)</f>
+        <v>7 TQ</v>
+      </c>
+      <c r="E13" s="1">
+        <f>MAX(F13,G13)</f>
         <v>7</v>
       </c>
-      <c r="G12" s="10">
+      <c r="F13" s="10">
         <f>TQ-1-SEG1PH_TQ-MIN(MAX(TQ-SEG1PH_TQ-8-1,2),8)</f>
         <v>7</v>
       </c>
-      <c r="H12" s="10">
+      <c r="G13" s="10">
         <f>MIN(MAX(ROUNDUP(PROPAGATION_TIME_DESIRED / TQ_TIME, 0), 1), 8)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
-        <f>E13-1</f>
+      <c r="B14" s="4">
+        <f>SEG1PH_TQ-1</f>
         <v>5</v>
       </c>
-      <c r="C13" s="8" t="str">
-        <f>VLOOKUP(B13,E26:F33,2)</f>
+      <c r="C14" s="8" t="str">
+        <f>VLOOKUP(B14,E27:F34,2)</f>
         <v>6 TQ</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E14" s="10">
         <f>MIN(MAX(FLOOR(TQ/2,1)-2,1),8)</f>
         <v>6</v>
       </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4">
-        <f>E14-1</f>
+      <c r="B15" s="4">
+        <f>SEG2PH_TQ-1</f>
         <v>1</v>
       </c>
-      <c r="C14" s="8" t="str">
-        <f>VLOOKUP(B14,E26:F33,2)</f>
+      <c r="C15" s="8" t="str">
+        <f>VLOOKUP(B15,E27:F34,2)</f>
         <v>2 TQ</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E15" s="10">
         <f>MIN(MAX(TQ-SEG1PH_TQ-PRSEG_TQ-1,1),8)</f>
         <v>2</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
-        <f>E15-1</f>
+      <c r="B16" s="4">
+        <f>SJW_TQ-1</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="str">
+        <f>VLOOKUP(B16,E27:F34,2)</f>
+        <v>1 TQ</v>
+      </c>
+      <c r="E16" s="30">
+        <f>MIN(F16,G16,SEG1PH_TQ,SEG2PH_TQ)</f>
         <v>1</v>
       </c>
-      <c r="C15" s="8" t="str">
-        <f>VLOOKUP(B15,E26:F33,2)</f>
-        <v>2 TQ</v>
-      </c>
-      <c r="E15" s="10">
-        <f>MIN(F15,SEG1PH_TQ,SEG2PH_TQ)</f>
-        <v>2</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="F16" s="10">
         <f>MIN(MAX(FLOOR(PRSEG_TQ/2,1),1),4)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="G16" s="30">
+        <f>IF(TQ-PRSEG_TQ-SEG1PH_TQ-SEG2PH_TQ&gt;0,TQ-PRSEG_TQ-SEG1PH_TQ-SEG2PH_TQ,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="16">
-        <f>E17*1000000</f>
+      <c r="B18" s="16">
+        <f>E18*1000000</f>
         <v>0.5</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="E17" s="12">
+      <c r="C18" s="16"/>
+      <c r="E18" s="12">
         <f>2 * (BRP + 1) / FREQUENCY</f>
         <v>4.9999999999999998E-7</v>
       </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="16">
-        <f>E18*1000000</f>
+      <c r="B19" s="16">
+        <f>E19*1000000</f>
         <v>8</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="E18" s="12">
+      <c r="C19" s="16"/>
+      <c r="E19" s="12">
         <f>TQ*TQ_TIME</f>
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="16">
-        <f>E19*1000000</f>
+      <c r="B20" s="16">
+        <f>E20*1000000</f>
         <v>3.5</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="E19" s="12">
+      <c r="C20" s="16"/>
+      <c r="E20" s="12">
         <f>PRSEG_TQ*TQ_TIME</f>
         <v>3.4999999999999999E-6</v>
       </c>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1486,98 +1690,118 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="14">
-        <v>5.0000000000000001E-9</v>
-      </c>
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E24" s="14">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="14">
         <v>2.4999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="E26" s="11">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E27" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E28" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E29" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E30" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E31" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E32" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="5:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="E33" s="11">
+        <v>6</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="E34" s="11">
         <v>7</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
+  <conditionalFormatting sqref="B10:C10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="notEqual">
+      <formula>$B$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:C7">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notBetween">
+      <formula>-0.01</formula>
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:C6">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="notEqual">
+      <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
       <formula1>0</formula1>
       <formula2>31</formula2>
     </dataValidation>
@@ -1619,7 +1843,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6">
@@ -1648,7 +1872,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="13">
         <v>5000</v>
       </c>

</xml_diff>

<commit_message>
Refactoring and removing unsupported speed (due to high frequency clock).
</commit_message>
<xml_diff>
--- a/Firmware/Resources/CanBusSpeed.xlsx
+++ b/Firmware/Resources/CanBusSpeed.xlsx
@@ -597,7 +597,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1279,9 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1690,19 +1698,25 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
       <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notBetween">
       <formula>-0.01</formula>
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:C12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
+      <formula>1</formula>
+      <formula>63</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">

</xml_diff>